<commit_message>
Added FishStatJ global production data + pre_processing script
</commit_message>
<xml_diff>
--- a/FootPlus Annotations.xlsx
+++ b/FootPlus Annotations.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mattia\Desktop\Polimi\Magistrale\FootPlus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA048615-243D-4B4D-B1C4-EEF7DD083525}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37425485-15D7-4872-836F-BCF30549B5B0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="79">
   <si>
     <t>estratto o riflessione</t>
   </si>
@@ -1101,6 +1101,15 @@
   <si>
     <t>Pagina contenent svariati dataset. Ne ho spulciato qualcuno e la cosa interessante è che hanno una timeline costante (mese-anno), molto utile per un comparison temporale</t>
   </si>
+  <si>
+    <t>https://science.sciencemag.org/content/sci/359/6378/904.full.pdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Paper di ricerca su fishing e carbon footprint. Si basa sul dataset dei "vessel" che avevamo già visto. Se approfondito, potrebbe avere senso, il paper propone dei risultati che potrebbero tornarci utili se riusciamo a trovare e interpretare il dataset che hanno usato </t>
+  </si>
+  <si>
+    <t>PAPER + dataset</t>
+  </si>
 </sst>
 </file>
 
@@ -1338,7 +1347,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1436,15 +1445,16 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1457,16 +1467,18 @@
     <xf numFmtId="0" fontId="12" fillId="5" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Collegamento ipertestuale" xfId="1" builtinId="8"/>
@@ -1727,8 +1739,8 @@
   </sheetPr>
   <dimension ref="A1:AA1002"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="A43" sqref="A43"/>
+    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="A44" sqref="A44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2247,7 +2259,7 @@
       <c r="AA14" s="5"/>
     </row>
     <row r="15" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A15" s="39" t="s">
+      <c r="A15" s="40" t="s">
         <v>36</v>
       </c>
       <c r="B15" s="23"/>
@@ -2280,7 +2292,7 @@
       <c r="AA15" s="5"/>
     </row>
     <row r="16" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A16" s="40"/>
+      <c r="A16" s="41"/>
       <c r="B16" s="23"/>
       <c r="C16" s="22" t="s">
         <v>34</v>
@@ -2311,7 +2323,7 @@
       <c r="AA16" s="5"/>
     </row>
     <row r="17" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A17" s="40"/>
+      <c r="A17" s="41"/>
       <c r="B17" s="23"/>
       <c r="C17" s="22" t="s">
         <v>33</v>
@@ -2342,7 +2354,7 @@
       <c r="AA17" s="5"/>
     </row>
     <row r="18" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A18" s="40"/>
+      <c r="A18" s="41"/>
       <c r="B18" s="23"/>
       <c r="C18" s="22" t="s">
         <v>32</v>
@@ -2373,7 +2385,7 @@
       <c r="AA18" s="5"/>
     </row>
     <row r="19" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A19" s="40"/>
+      <c r="A19" s="41"/>
       <c r="B19" s="23"/>
       <c r="C19" s="22" t="s">
         <v>31</v>
@@ -2404,7 +2416,7 @@
       <c r="AA19" s="5"/>
     </row>
     <row r="20" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A20" s="40"/>
+      <c r="A20" s="41"/>
       <c r="B20" s="24"/>
       <c r="C20" s="32" t="s">
         <v>30</v>
@@ -2435,17 +2447,17 @@
       <c r="AA20" s="5"/>
     </row>
     <row r="21" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="38" t="s">
+      <c r="A21" s="39" t="s">
         <v>66</v>
       </c>
-      <c r="B21" s="37" t="s">
+      <c r="B21" s="45" t="s">
         <v>65</v>
       </c>
       <c r="C21" s="29" t="s">
         <v>64</v>
       </c>
       <c r="D21" s="27"/>
-      <c r="E21" s="41" t="s">
+      <c r="E21" s="42" t="s">
         <v>67</v>
       </c>
       <c r="F21" s="5"/>
@@ -2472,13 +2484,13 @@
       <c r="AA21" s="5"/>
     </row>
     <row r="22" spans="1:27" ht="15" x14ac:dyDescent="0.25">
-      <c r="A22" s="38"/>
-      <c r="B22" s="37"/>
+      <c r="A22" s="39"/>
+      <c r="B22" s="45"/>
       <c r="C22" s="29" t="s">
         <v>63</v>
       </c>
       <c r="D22" s="27"/>
-      <c r="E22" s="35"/>
+      <c r="E22" s="43"/>
       <c r="F22" s="5"/>
       <c r="G22" s="5"/>
       <c r="H22" s="5"/>
@@ -2503,15 +2515,15 @@
       <c r="AA22" s="5"/>
     </row>
     <row r="23" spans="1:27" ht="15" x14ac:dyDescent="0.25">
-      <c r="A23" s="38"/>
-      <c r="B23" s="37" t="s">
+      <c r="A23" s="39"/>
+      <c r="B23" s="45" t="s">
         <v>62</v>
       </c>
       <c r="C23" s="29" t="s">
         <v>59</v>
       </c>
       <c r="D23" s="27"/>
-      <c r="E23" s="35"/>
+      <c r="E23" s="43"/>
       <c r="F23" s="5"/>
       <c r="G23" s="5"/>
       <c r="H23" s="5"/>
@@ -2536,13 +2548,13 @@
       <c r="AA23" s="5"/>
     </row>
     <row r="24" spans="1:27" ht="15" x14ac:dyDescent="0.25">
-      <c r="A24" s="38"/>
-      <c r="B24" s="37"/>
+      <c r="A24" s="39"/>
+      <c r="B24" s="45"/>
       <c r="C24" s="29" t="s">
         <v>60</v>
       </c>
       <c r="D24" s="27"/>
-      <c r="E24" s="35"/>
+      <c r="E24" s="43"/>
       <c r="F24" s="5"/>
       <c r="G24" s="5"/>
       <c r="H24" s="5"/>
@@ -2567,13 +2579,13 @@
       <c r="AA24" s="5"/>
     </row>
     <row r="25" spans="1:27" ht="15" x14ac:dyDescent="0.25">
-      <c r="A25" s="38"/>
-      <c r="B25" s="37"/>
+      <c r="A25" s="39"/>
+      <c r="B25" s="45"/>
       <c r="C25" s="29" t="s">
         <v>61</v>
       </c>
       <c r="D25" s="27"/>
-      <c r="E25" s="35"/>
+      <c r="E25" s="43"/>
       <c r="F25" s="5"/>
       <c r="G25" s="5"/>
       <c r="H25" s="5"/>
@@ -2598,7 +2610,7 @@
       <c r="AA25" s="5"/>
     </row>
     <row r="26" spans="1:27" ht="15" x14ac:dyDescent="0.2">
-      <c r="A26" s="38"/>
+      <c r="A26" s="39"/>
       <c r="B26" s="33" t="s">
         <v>58</v>
       </c>
@@ -2606,7 +2618,7 @@
         <v>57</v>
       </c>
       <c r="D26" s="27"/>
-      <c r="E26" s="35"/>
+      <c r="E26" s="43"/>
       <c r="F26" s="5"/>
       <c r="G26" s="5"/>
       <c r="H26" s="5"/>
@@ -2631,15 +2643,15 @@
       <c r="AA26" s="5"/>
     </row>
     <row r="27" spans="1:27" ht="15" x14ac:dyDescent="0.25">
-      <c r="A27" s="38"/>
-      <c r="B27" s="37" t="s">
+      <c r="A27" s="39"/>
+      <c r="B27" s="45" t="s">
         <v>51</v>
       </c>
       <c r="C27" s="29" t="s">
         <v>48</v>
       </c>
       <c r="D27" s="27"/>
-      <c r="E27" s="35"/>
+      <c r="E27" s="43"/>
       <c r="F27" s="5"/>
       <c r="G27" s="5"/>
       <c r="H27" s="5"/>
@@ -2664,13 +2676,13 @@
       <c r="AA27" s="5"/>
     </row>
     <row r="28" spans="1:27" ht="15" x14ac:dyDescent="0.25">
-      <c r="A28" s="38"/>
-      <c r="B28" s="37"/>
+      <c r="A28" s="39"/>
+      <c r="B28" s="45"/>
       <c r="C28" s="29" t="s">
         <v>49</v>
       </c>
       <c r="D28" s="27"/>
-      <c r="E28" s="35"/>
+      <c r="E28" s="43"/>
       <c r="F28" s="5"/>
       <c r="G28" s="5"/>
       <c r="H28" s="5"/>
@@ -2695,13 +2707,13 @@
       <c r="AA28" s="5"/>
     </row>
     <row r="29" spans="1:27" ht="15" x14ac:dyDescent="0.25">
-      <c r="A29" s="38"/>
-      <c r="B29" s="37"/>
+      <c r="A29" s="39"/>
+      <c r="B29" s="45"/>
       <c r="C29" s="29" t="s">
         <v>50</v>
       </c>
       <c r="D29" s="27"/>
-      <c r="E29" s="35"/>
+      <c r="E29" s="43"/>
       <c r="F29" s="5"/>
       <c r="G29" s="5"/>
       <c r="H29" s="5"/>
@@ -2726,7 +2738,7 @@
       <c r="AA29" s="5"/>
     </row>
     <row r="30" spans="1:27" ht="15" x14ac:dyDescent="0.25">
-      <c r="A30" s="38"/>
+      <c r="A30" s="39"/>
       <c r="B30" s="33" t="s">
         <v>54</v>
       </c>
@@ -2734,7 +2746,7 @@
         <v>53</v>
       </c>
       <c r="D30" s="27"/>
-      <c r="E30" s="35"/>
+      <c r="E30" s="43"/>
       <c r="F30" s="5"/>
       <c r="G30" s="5"/>
       <c r="H30" s="5"/>
@@ -2759,7 +2771,7 @@
       <c r="AA30" s="5"/>
     </row>
     <row r="31" spans="1:27" ht="15" x14ac:dyDescent="0.25">
-      <c r="A31" s="38"/>
+      <c r="A31" s="39"/>
       <c r="B31" s="33" t="s">
         <v>52</v>
       </c>
@@ -2767,7 +2779,7 @@
         <v>39</v>
       </c>
       <c r="D31" s="27"/>
-      <c r="E31" s="35"/>
+      <c r="E31" s="43"/>
       <c r="F31" s="5"/>
       <c r="G31" s="5"/>
       <c r="H31" s="5"/>
@@ -2792,7 +2804,7 @@
       <c r="AA31" s="5"/>
     </row>
     <row r="32" spans="1:27" ht="15" x14ac:dyDescent="0.25">
-      <c r="A32" s="38"/>
+      <c r="A32" s="39"/>
       <c r="B32" s="33" t="s">
         <v>47</v>
       </c>
@@ -2800,7 +2812,7 @@
         <v>37</v>
       </c>
       <c r="D32" s="27"/>
-      <c r="E32" s="35"/>
+      <c r="E32" s="43"/>
       <c r="F32" s="5"/>
       <c r="G32" s="5"/>
       <c r="H32" s="5"/>
@@ -2825,7 +2837,7 @@
       <c r="AA32" s="5"/>
     </row>
     <row r="33" spans="1:27" ht="15" x14ac:dyDescent="0.25">
-      <c r="A33" s="38"/>
+      <c r="A33" s="39"/>
       <c r="B33" s="33" t="s">
         <v>56</v>
       </c>
@@ -2833,7 +2845,7 @@
         <v>55</v>
       </c>
       <c r="D33" s="27"/>
-      <c r="E33" s="35"/>
+      <c r="E33" s="43"/>
       <c r="F33" s="5"/>
       <c r="G33" s="5"/>
       <c r="H33" s="5"/>
@@ -2858,15 +2870,15 @@
       <c r="AA33" s="5"/>
     </row>
     <row r="34" spans="1:27" ht="15" x14ac:dyDescent="0.25">
-      <c r="A34" s="38"/>
-      <c r="B34" s="37" t="s">
+      <c r="A34" s="39"/>
+      <c r="B34" s="45" t="s">
         <v>46</v>
       </c>
       <c r="C34" s="31" t="s">
         <v>45</v>
       </c>
       <c r="D34" s="27"/>
-      <c r="E34" s="35"/>
+      <c r="E34" s="43"/>
       <c r="F34" s="5"/>
       <c r="G34" s="5"/>
       <c r="H34" s="5"/>
@@ -2891,13 +2903,13 @@
       <c r="AA34" s="5"/>
     </row>
     <row r="35" spans="1:27" ht="15" x14ac:dyDescent="0.25">
-      <c r="A35" s="38"/>
-      <c r="B35" s="37"/>
+      <c r="A35" s="39"/>
+      <c r="B35" s="45"/>
       <c r="C35" s="31" t="s">
         <v>44</v>
       </c>
       <c r="D35" s="27"/>
-      <c r="E35" s="35"/>
+      <c r="E35" s="43"/>
       <c r="F35" s="5"/>
       <c r="G35" s="5"/>
       <c r="H35" s="5"/>
@@ -2922,13 +2934,13 @@
       <c r="AA35" s="5"/>
     </row>
     <row r="36" spans="1:27" ht="15" x14ac:dyDescent="0.25">
-      <c r="A36" s="38"/>
-      <c r="B36" s="37"/>
+      <c r="A36" s="39"/>
+      <c r="B36" s="45"/>
       <c r="C36" s="31" t="s">
         <v>43</v>
       </c>
       <c r="D36" s="27"/>
-      <c r="E36" s="35"/>
+      <c r="E36" s="43"/>
       <c r="F36" s="5"/>
       <c r="G36" s="5"/>
       <c r="H36" s="5"/>
@@ -2953,13 +2965,13 @@
       <c r="AA36" s="5"/>
     </row>
     <row r="37" spans="1:27" ht="15" x14ac:dyDescent="0.25">
-      <c r="A37" s="38"/>
-      <c r="B37" s="37"/>
+      <c r="A37" s="39"/>
+      <c r="B37" s="45"/>
       <c r="C37" s="31" t="s">
         <v>42</v>
       </c>
       <c r="D37" s="27"/>
-      <c r="E37" s="35"/>
+      <c r="E37" s="43"/>
       <c r="F37" s="5"/>
       <c r="G37" s="5"/>
       <c r="H37" s="5"/>
@@ -2984,13 +2996,13 @@
       <c r="AA37" s="5"/>
     </row>
     <row r="38" spans="1:27" ht="15" x14ac:dyDescent="0.25">
-      <c r="A38" s="38"/>
-      <c r="B38" s="37"/>
+      <c r="A38" s="39"/>
+      <c r="B38" s="45"/>
       <c r="C38" s="31" t="s">
         <v>41</v>
       </c>
       <c r="D38" s="27"/>
-      <c r="E38" s="35"/>
+      <c r="E38" s="43"/>
       <c r="F38" s="5"/>
       <c r="G38" s="5"/>
       <c r="H38" s="5"/>
@@ -3015,7 +3027,7 @@
       <c r="AA38" s="5"/>
     </row>
     <row r="39" spans="1:27" ht="15" x14ac:dyDescent="0.25">
-      <c r="A39" s="38"/>
+      <c r="A39" s="39"/>
       <c r="B39" s="33" t="s">
         <v>40</v>
       </c>
@@ -3023,7 +3035,7 @@
         <v>39</v>
       </c>
       <c r="D39" s="27"/>
-      <c r="E39" s="35"/>
+      <c r="E39" s="43"/>
       <c r="F39" s="5"/>
       <c r="G39" s="5"/>
       <c r="H39" s="5"/>
@@ -3048,7 +3060,7 @@
       <c r="AA39" s="5"/>
     </row>
     <row r="40" spans="1:27" ht="15" x14ac:dyDescent="0.25">
-      <c r="A40" s="38"/>
+      <c r="A40" s="39"/>
       <c r="B40" s="33" t="s">
         <v>38</v>
       </c>
@@ -3056,7 +3068,7 @@
         <v>37</v>
       </c>
       <c r="D40" s="27"/>
-      <c r="E40" s="36"/>
+      <c r="E40" s="44"/>
       <c r="F40" s="5"/>
       <c r="G40" s="5"/>
       <c r="H40" s="5"/>
@@ -3085,11 +3097,11 @@
         <v>68</v>
       </c>
       <c r="B41" s="30"/>
-      <c r="C41" s="44" t="s">
+      <c r="C41" s="37" t="s">
         <v>70</v>
       </c>
       <c r="D41" s="27"/>
-      <c r="E41" s="43" t="s">
+      <c r="E41" s="36" t="s">
         <v>69</v>
       </c>
       <c r="F41" s="5"/>
@@ -3120,11 +3132,11 @@
         <v>72</v>
       </c>
       <c r="B42" s="30"/>
-      <c r="C42" s="45" t="s">
+      <c r="C42" s="38" t="s">
         <v>73</v>
       </c>
       <c r="D42" s="27"/>
-      <c r="E42" s="42" t="s">
+      <c r="E42" s="35" t="s">
         <v>71</v>
       </c>
       <c r="F42" s="5"/>
@@ -3155,11 +3167,11 @@
         <v>36</v>
       </c>
       <c r="B43" s="30"/>
-      <c r="C43" s="45" t="s">
+      <c r="C43" s="38" t="s">
         <v>75</v>
       </c>
       <c r="D43" s="27"/>
-      <c r="E43" s="42" t="s">
+      <c r="E43" s="35" t="s">
         <v>74</v>
       </c>
       <c r="F43" s="5"/>
@@ -3185,12 +3197,18 @@
       <c r="Z43" s="5"/>
       <c r="AA43" s="5"/>
     </row>
-    <row r="44" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A44" s="28"/>
+    <row r="44" spans="1:27" ht="56.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="28" t="s">
+        <v>78</v>
+      </c>
       <c r="B44" s="30"/>
-      <c r="C44" s="30"/>
+      <c r="C44" s="46" t="s">
+        <v>77</v>
+      </c>
       <c r="D44" s="27"/>
-      <c r="E44" s="20"/>
+      <c r="E44" s="20" t="s">
+        <v>76</v>
+      </c>
       <c r="F44" s="5"/>
       <c r="G44" s="5"/>
       <c r="H44" s="5"/>

</xml_diff>